<commit_message>
Fixed some data stuff
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Uni\Programming\C\DSA\Project\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC8080E-7B98-42DE-BEB1-898DEED62878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="30612" yWindow="2136" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -82,19 +91,21 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -104,50 +115,53 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
     <dxf>
-      <font/>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFB7E1CD"/>
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
-      <border/>
     </dxf>
   </dxfs>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -337,20 +351,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -370,7 +389,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I2" s="1" t="s">
         <v>6</v>
       </c>
@@ -385,194 +404,194 @@
       </c>
       <c r="O2" s="1"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F3" s="1">
-        <v>1.234234121E9</v>
+        <v>1234234121</v>
       </c>
       <c r="I3" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J3" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="L3" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M3" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O3" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F4" s="1">
-        <v>1.234567812E9</v>
+        <v>1234567812</v>
       </c>
       <c r="I4" s="1">
-        <v>2.0</v>
+        <v>0</v>
       </c>
       <c r="J4" s="1">
-        <v>8.0</v>
+        <v>10</v>
       </c>
       <c r="L4" s="1">
-        <v>0.0</v>
+        <v>2</v>
       </c>
       <c r="M4" s="1">
-        <v>10.0</v>
+        <v>8</v>
       </c>
       <c r="O4" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="F5" s="2">
-        <v>1.343251452313E12</v>
+        <v>1343251452313</v>
       </c>
       <c r="I5" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J5" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L5" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="M5" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="O5" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I6" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J6" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="L6" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M6" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="O6" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B7" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F7" s="1">
-        <v>7.01203042303212E14</v>
+        <v>701203042303212</v>
       </c>
       <c r="I7" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J7" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="M7" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="O7" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B8" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J8" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L8" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M8" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="O8" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="9">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B9" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="I9" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J9" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="L9" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M9" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="O9" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J10" s="1">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="L10" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M10" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="O10" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="F11" s="1"/>
       <c r="I11" s="1"/>
@@ -580,378 +599,378 @@
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F14" s="1">
-        <v>1.2453421545E10</v>
+        <v>12453421545</v>
       </c>
       <c r="I14" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="L14" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="M14" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="O14" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B15" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="F15" s="1">
-        <v>1.4523678945E10</v>
+        <v>14523678945</v>
       </c>
       <c r="I15" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J15" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="L15" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M15" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="O15" s="1">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B16" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="F16" s="1">
-        <v>1.4352654323546E13</v>
+        <v>14352654323546</v>
       </c>
       <c r="I16" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J16" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="L16" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="M16" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="O16" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B17" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="I17" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="L17" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M17" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="O17" s="1">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B18" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I18" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="J18" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L18" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="M18" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="O18" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B19" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>14</v>
       </c>
       <c r="I19" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J19" s="1">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="L19" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M19" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="O19" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B20" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="J20" s="1">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="L20" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M20" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="O20" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>16</v>
       </c>
       <c r="I21" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J21" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M21" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="O21" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="23">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F23" s="1">
-        <v>1.432431245E9</v>
+        <v>1432431245</v>
       </c>
       <c r="I23" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J23" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L23" s="1">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="M23" s="1">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="O23" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B24" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="F24" s="1">
-        <v>1.432567821E9</v>
+        <v>1432567821</v>
       </c>
       <c r="I24" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="J24" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="L24" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M24" s="1">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="O24" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B25" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="F25" s="1">
-        <v>1.32451345212E11</v>
+        <v>132451345212</v>
       </c>
       <c r="I25" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="J25" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="L25" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="M25" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="O25" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>17</v>
       </c>
       <c r="I26" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J26" s="1">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="L26" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="M26" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="O26" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="I27" s="1">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="J27" s="1">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="L27" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="M27" s="1">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="O27" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I28" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J28" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="L28" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M28" s="1">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="O28" s="1">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>20</v>
       </c>
       <c r="I29" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="J29" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="L29" s="1">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="M29" s="1">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="O29" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I30" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="J30" s="1">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="L30" s="1">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="M30" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="O30" s="1">
-        <v>16.0</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -960,6 +979,6 @@
       <formula>LEN(TRIM(B11))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>